<commit_message>
[Update] Lobby Server 예제 업데이트
</commit_message>
<xml_diff>
--- a/example/MetaData/Event.xlsx
+++ b/example/MetaData/Event.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>item_count</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,10 @@
   </si>
   <si>
     <t>mail_expire_day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>event</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -407,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -472,7 +476,41 @@
         <v>100001</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>100002</v>
+      </c>
+      <c r="E4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>100003</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>